<commit_message>
DA delta working. Implementing TM delta
</commit_message>
<xml_diff>
--- a/my_study.xlsx
+++ b/my_study.xlsx
@@ -425,7 +425,7 @@
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="2" min="2" width="14.88671875"/>
     <col customWidth="1" max="13" min="13" width="14.88671875"/>
@@ -8446,7 +8446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H132"/>
+  <dimension ref="A1:H136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12018,6 +12018,114 @@
         </is>
       </c>
       <c r="H132" t="inlineStr">
+        <is>
+          <t>THEBRAIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>15-10-2019</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>18:24:25</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>(): Launched: Examining ['c']</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>oliver</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>THEBRAIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>15-10-2019</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>18:24:25</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>(): Completed. Deidentified 0, failed 0</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>oliver</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>THEBRAIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>16-10-2019</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>08:34:27</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>(): Launched: Examining ['C:\\Users\\oliver\\Documents\\pycode\\Batch-DICOM-Anonymiser\\sample_1']</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>oliver</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>THEBRAIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>16-10-2019</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>08:34:37</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>(): Completed. Deidentified 0, failed 0</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>oliver</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
         <is>
           <t>THEBRAIN</t>
         </is>
@@ -12034,13 +12142,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="5" min="5" width="21.88671875"/>
     <col bestFit="1" customWidth="1" max="11" min="11" width="12.88671875"/>
@@ -12437,6 +12545,7 @@
         </is>
       </c>
     </row>
+    <row r="31"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>